<commit_message>
Update LHJ data and documentation
</commit_message>
<xml_diff>
--- a/LHJ Data/finalPopData/Data-Dictionary.xlsx
+++ b/LHJ Data/finalPopData/Data-Dictionary.xlsx
@@ -1,82 +1,92 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FusionData\Population Task Force\LHJ Data\finalPopData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB1A6917-BE86-4634-8ADF-0AFD430EF118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="19860" yWindow="1725" windowWidth="17220" windowHeight="18270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t xml:space="preserve">Column</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of Unique Values</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">county_lhj</t>
-  </si>
-  <si>
-    <t xml:space="preserve">character</t>
-  </si>
-  <si>
-    <t xml:space="preserve">58 California Counties (Alameda, Alpine, etc), 3 city jurisdictions (Berkeley, Long Beach, Pasadena), Alameda HD, and Los Angeles HD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">integer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Annual; Ranges from 2000 to 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sex at birth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Single years of age; Ages 100 and over are aggregated into '100+'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">raceEth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Race/Ethnicity; Single races are defined as race alone and not Hispanic; Multi-Race is two or more races and not-Hispanic; Note: AI/AN = American Indian/Alaskan Native; NH/PI = Native Hawaiian/Pacific Islander</t>
-  </si>
-  <si>
-    <t xml:space="preserve">population</t>
-  </si>
-  <si>
-    <t xml:space="preserve">double</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Population estimates; data file 'lhj-population-ars-adjJuly' contains population estimates that are adjusted to July 1st estimates; 'lhj-population-ars' contains non-adjusted population estimates</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>Data Type</t>
+  </si>
+  <si>
+    <t>Number of Unique Values</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>county_lhj</t>
+  </si>
+  <si>
+    <t>character</t>
+  </si>
+  <si>
+    <t>58 California Counties (Alameda, Alpine, etc), 3 city jurisdictions (Berkeley, Long Beach, Pasadena), Alameda HD, and Los Angeles HD</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>Annual; Ranges from 2000 to 2023</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>Sex at birth</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>Race/Ethnicity; Single races are defined as race alone and not Hispanic; Multi-Race is two or more races and not-Hispanic; Note: AI/AN = American Indian/Alaskan Native; NH/PI = Native Hawaiian/Pacific Islander</t>
+  </si>
+  <si>
+    <t>population</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>Single years of age; Ages 100 and over are aggregated into '100'</t>
+  </si>
+  <si>
+    <t>race_eth</t>
+  </si>
+  <si>
+    <t>Population estimates; data file 'lhj-pop-ars-2000-cy' contains population estimates from 2000-2023, and is recommended to use for trends; 'lhj-pop-ars-2020-cy' contains population estimates from 2020-2023, and is recommended to use for displaying recent years of data.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -85,10 +95,10 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <b/>
     </font>
   </fonts>
   <fills count="3">
@@ -116,24 +126,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:D7" totalsRowCount="0" totalsRowShown="0">
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:D7" totalsRowShown="0">
   <tableColumns count="4">
-    <tableColumn id="1" name="Column"/>
-    <tableColumn id="2" name="Data Type"/>
-    <tableColumn id="3" name="Number of Unique Values"/>
-    <tableColumn id="4" name="Description"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Data Type"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Number of Unique Values"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -417,22 +439,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="0" tabSelected="true">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="11.71" hidden="0" customWidth="1"/>
-    <col min="3" max="3" width="24.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="200.71" hidden="0" customWidth="1"/>
+    <col min="1" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="200.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -446,93 +468,92 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>63</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>24</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>2</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="n">
+        <v>16</v>
+      </c>
+      <c r="C5">
         <v>101</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>7</v>
       </c>
       <c r="D6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7"/>
-      <c r="D7" t="s">
-        <v>18</v>
+      <c r="D7" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update LHJ Population data with new DOF intercensal and P3
</commit_message>
<xml_diff>
--- a/LHJ Data/finalPopData/Data-Dictionary.xlsx
+++ b/LHJ Data/finalPopData/Data-Dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FusionData\Population Task Force\LHJ Data\finalPopData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB1A6917-BE86-4634-8ADF-0AFD430EF118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B894C693-6989-458A-B61F-2AF7F56B88C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19860" yWindow="1725" windowWidth="17220" windowHeight="18270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3900" yWindow="3900" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,38 +20,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Column</t>
   </si>
   <si>
-    <t>Data Type</t>
-  </si>
-  <si>
-    <t>Number of Unique Values</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
     <t>county_lhj</t>
   </si>
   <si>
-    <t>character</t>
-  </si>
-  <si>
     <t>58 California Counties (Alameda, Alpine, etc), 3 city jurisdictions (Berkeley, Long Beach, Pasadena), Alameda HD, and Los Angeles HD</t>
   </si>
   <si>
     <t>year</t>
   </si>
   <si>
-    <t>integer</t>
-  </si>
-  <si>
-    <t>Annual; Ranges from 2000 to 2023</t>
-  </si>
-  <si>
     <t>sex</t>
   </si>
   <si>
@@ -67,19 +52,16 @@
     <t>population</t>
   </si>
   <si>
-    <t>double</t>
-  </si>
-  <si>
-    <t>numeric</t>
-  </si>
-  <si>
     <t>Single years of age; Ages 100 and over are aggregated into '100'</t>
   </si>
   <si>
     <t>race_eth</t>
   </si>
   <si>
-    <t>Population estimates; data file 'lhj-pop-ars-2000-cy' contains population estimates from 2000-2023, and is recommended to use for trends; 'lhj-pop-ars-2020-cy' contains population estimates from 2020-2023, and is recommended to use for displaying recent years of data.</t>
+    <t>Annual; Ranges from 2000 to 2024</t>
+  </si>
+  <si>
+    <t>Population estimates</t>
   </si>
 </sst>
 </file>
@@ -150,11 +132,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:D7" totalsRowShown="0">
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:B7" totalsRowShown="0">
+  <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Data Type"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Number of Unique Values"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -440,113 +420,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D7" sqref="D7"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" customWidth="1"/>
-    <col min="4" max="4" width="200.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="200.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
-        <v>63</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C3">
-        <v>24</v>
-      </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5">
-        <v>101</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="B7" s="2" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>